<commit_message>
updated formatting of spreadsheets in Export class and in current xlsx files
</commit_message>
<xml_diff>
--- a/excel/220503.xlsx
+++ b/excel/220503.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messiosa\Documents\work\data_projects\mp_second_jobs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CDB4F4-9E8D-45C9-BEDF-8A654AFB2292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A506C14-24AF-4E20-AFD6-CDEFFC86D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7831" uniqueCount="3047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7831" uniqueCount="3046">
   <si>
     <t>Political Party</t>
   </si>
@@ -9084,21 +9084,12 @@
     <t>Sheet 1: MP Overview - Totals of second job MP earnings and hours worked for the year-to-date</t>
   </si>
   <si>
-    <t>Total Earnings YTD (£) - Total declared employment earnings outside of MP work in the last year</t>
-  </si>
-  <si>
-    <t>Total Hours Worked YTD - Total declared hours spent working outside of MP work in the last year</t>
-  </si>
-  <si>
     <t>Basic MP Salary (2020-21) - Salary received as a Member of Parliament in 2020-21 (not included in Total Earnings YTD)</t>
   </si>
   <si>
     <t>LALP (2020-21) - Sum received as a London Area Living Payment adjustment in 2020-21</t>
   </si>
   <si>
-    <t>Date Assumed Office and Years in Office</t>
-  </si>
-  <si>
     <t>Majority - % majority won in last election</t>
   </si>
   <si>
@@ -9123,9 +9114,6 @@
     <t>Hours Worked YTD - Approximation of % of hours worked in the last year (e.g. annual time commitment * % of year elapsed)</t>
   </si>
   <si>
-    <t>Original text - Original text from the Register of MP Financial Interests</t>
-  </si>
-  <si>
     <t>Source - Hyperlink to the corresponding record in the Register of MP Financial Interests</t>
   </si>
   <si>
@@ -9163,6 +9151,15 @@
   </si>
   <si>
     <t>Expenses (2020-21) - Expenses claimed in 2020-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Secondary Earnings YTD (£) - Total declared employment earnings outside of MP work in the last year</t>
+  </si>
+  <si>
+    <t>Secondary Hours Worked YTD - Total declared hours spent working outside of MP work in the last year</t>
   </si>
 </sst>
 </file>
@@ -9620,10 +9617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9648,136 +9645,136 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3020</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3021</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>3022</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3023</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>3045</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>3046</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>3024</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>3025</v>
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>3043</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>3026</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>3027</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>3028</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>3029</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>3030</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>3031</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>3032</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>3033</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>3034</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>3035</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>3036</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>3037</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>3038</v>
+        <v>3035</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>3039</v>
+        <v>3036</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>3040</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>3041</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>3042</v>
+        <v>3038</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A30" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A32" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A33" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A31" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A32" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9818,10 +9815,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>3043</v>
+        <v>3039</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>3044</v>
+        <v>3040</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
@@ -36191,7 +36188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I923"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
updated edgedriver to v103 + scraped 220516, 220530, 220613
</commit_message>
<xml_diff>
--- a/excel/220503.xlsx
+++ b/excel/220503.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messiosa\Documents\work\data_projects\mp_second_jobs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A506C14-24AF-4E20-AFD6-CDEFFC86D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22F2A60-D4EB-4BDF-89D2-338CA2805BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -9620,7 +9620,7 @@
   <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9785,10 +9785,10 @@
   <dimension ref="A1:M650"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36189,10 +36189,10 @@
   <dimension ref="A1:I923"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>